<commit_message>
Updated and verified category 2 test cases after implementing the TZ_NAME validation
</commit_message>
<xml_diff>
--- a/docs/packages/CDVM/test cases/verification_templates/category_2_DVM_issue_verification.xlsx
+++ b/docs/packages/CDVM/test cases/verification_templates/category_2_DVM_issue_verification.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6465" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6465"/>
   </bookViews>
   <sheets>
     <sheet name="CCD_CRUISE_SUMM_ERR_V" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="121">
   <si>
     <t>CRUISE_NAME</t>
   </si>
@@ -367,6 +367,24 @@
   </si>
   <si>
     <t>The Cruise (TC0201) has a Cruise Leg (TC0201_LEGI) on the Vessel (Townsend Cromwell) with a Start Date (01/21/2002) and End Date (02/14/2002) that does not have at least one data set associated with it</t>
+  </si>
+  <si>
+    <t>Invalid Leg Timezone</t>
+  </si>
+  <si>
+    <t>The leg's timezone does not match a timezone value in the Oracle reference list</t>
+  </si>
+  <si>
+    <t>The Cruise (HI1001) has a Cruise Leg (HI1001_LEGII) on the Vessel (Hi'ialakai) with a Start Date (06/15/2010) and End Date (07/03/2010) has an invalid timezone (ASDF JKL;) specified for it</t>
+  </si>
+  <si>
+    <t>INV_TZ_NAME_YN</t>
+  </si>
+  <si>
+    <t>The Cruise (RL-17-05) has a Cruise Leg (RL-17-05 Leg 2) on the Vessel (Reuben Lasker) with a Start Date (09/11/2017) and End Date (09/30/2017) has an invalid timezone (+09:00) specified for it</t>
+  </si>
+  <si>
+    <t>The Cruise (SE-04-11) has a Cruise Leg (OES0411_LEGII) on the Vessel (Oscar Elton Sette) with a Start Date (09/08/2005) and End Date (09/13/2005) has an invalid timezone (Hawaii Standard Time) specified for it</t>
   </si>
 </sst>
 </file>
@@ -694,11 +712,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31:XFD31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,53 +888,53 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:7" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
         <v>25</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" t="s">
-        <v>84</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>43</v>
       </c>
@@ -927,19 +945,19 @@
         <v>84</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>32</v>
+        <v>78</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="G10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -947,22 +965,22 @@
         <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="D11" t="s">
-        <v>108</v>
-      </c>
-      <c r="E11" t="s">
-        <v>109</v>
-      </c>
-      <c r="F11" t="s">
-        <v>110</v>
+        <v>31</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="G11" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -973,19 +991,19 @@
         <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>46</v>
+        <v>108</v>
+      </c>
+      <c r="E12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F12" t="s">
+        <v>110</v>
       </c>
       <c r="G12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -996,19 +1014,19 @@
         <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>75</v>
-      </c>
-      <c r="E13" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" t="s">
-        <v>99</v>
+        <v>26</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="G13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -1019,42 +1037,42 @@
         <v>25</v>
       </c>
       <c r="D14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" t="s">
+        <v>99</v>
+      </c>
+      <c r="G14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" t="s">
         <v>76</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -1062,50 +1080,50 @@
         <v>48</v>
       </c>
       <c r="C16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" t="s">
         <v>25</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G17" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>58</v>
-      </c>
-      <c r="B17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" t="s">
-        <v>84</v>
-      </c>
-      <c r="D17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G17" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
         <v>84</v>
@@ -1117,13 +1135,13 @@
         <v>78</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -1134,65 +1152,65 @@
         <v>84</v>
       </c>
       <c r="D19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" t="s">
         <v>60</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G20" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="21" spans="1:7" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" t="s">
-        <v>108</v>
-      </c>
-      <c r="E20" t="s">
-        <v>109</v>
-      </c>
-      <c r="F20" t="s">
-        <v>112</v>
-      </c>
-      <c r="G20" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>64</v>
-      </c>
-      <c r="B21" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C21" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -1203,116 +1221,116 @@
         <v>25</v>
       </c>
       <c r="D22" t="s">
-        <v>75</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>74</v>
+        <v>108</v>
+      </c>
+      <c r="E22" t="s">
+        <v>109</v>
+      </c>
+      <c r="F22" t="s">
+        <v>112</v>
       </c>
       <c r="G22" t="s">
-        <v>35</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="C23" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="D23" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="G23" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s">
         <v>25</v>
       </c>
       <c r="D24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="G24" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s">
         <v>84</v>
       </c>
       <c r="D25" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G25" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>104</v>
-      </c>
-      <c r="B26" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" t="s">
-        <v>25</v>
-      </c>
-      <c r="D26" t="s">
-        <v>108</v>
-      </c>
-      <c r="E26" t="s">
-        <v>109</v>
-      </c>
-      <c r="F26" t="s">
-        <v>113</v>
-      </c>
-      <c r="G26" t="s">
-        <v>111</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>67</v>
+        <v>101</v>
       </c>
       <c r="B27" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="C27" t="s">
         <v>25</v>
@@ -1324,95 +1342,164 @@
         <v>38</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G27" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>69</v>
+        <v>104</v>
+      </c>
+      <c r="B28" t="s">
+        <v>54</v>
       </c>
       <c r="C28" t="s">
         <v>84</v>
       </c>
       <c r="D28" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>104</v>
+      </c>
+      <c r="B29" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" t="s">
+        <v>108</v>
+      </c>
+      <c r="E29" t="s">
+        <v>109</v>
+      </c>
+      <c r="F29" t="s">
+        <v>113</v>
+      </c>
+      <c r="G29" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" t="s">
+        <v>77</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31" t="s">
         <v>14</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G31" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="32" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>69</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C32" t="s">
         <v>84</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D32" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G32" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="33" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>71</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B33" t="s">
         <v>72</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C33" t="s">
         <v>84</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D33" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G33" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>71</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B34" t="s">
         <v>72</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C34" t="s">
         <v>25</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D34" t="s">
         <v>108</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G34" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1428,10 +1515,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G31"/>
+      <selection sqref="A1:G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1608,42 +1695,42 @@
         <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>115</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
+        <v>116</v>
       </c>
       <c r="F8" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="G8" t="s">
-        <v>42</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="E9" t="s">
-        <v>78</v>
+        <v>41</v>
       </c>
       <c r="F9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G9" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1657,16 +1744,16 @@
         <v>84</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>78</v>
       </c>
       <c r="F10" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="G10" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1677,19 +1764,19 @@
         <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="D11" t="s">
-        <v>108</v>
+        <v>31</v>
       </c>
       <c r="E11" t="s">
-        <v>109</v>
+        <v>32</v>
       </c>
       <c r="F11" t="s">
-        <v>110</v>
+        <v>45</v>
       </c>
       <c r="G11" t="s">
-        <v>111</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1703,16 +1790,16 @@
         <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>108</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>109</v>
       </c>
       <c r="F12" t="s">
-        <v>46</v>
+        <v>110</v>
       </c>
       <c r="G12" t="s">
-        <v>28</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1726,16 +1813,16 @@
         <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>75</v>
+        <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F13" t="s">
-        <v>99</v>
+        <v>46</v>
       </c>
       <c r="G13" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1749,39 +1836,39 @@
         <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="E15" t="s">
-        <v>78</v>
+        <v>36</v>
       </c>
       <c r="F15" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="G15" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1792,50 +1879,50 @@
         <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="D16" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="F16" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="G16" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="E17" t="s">
-        <v>78</v>
+        <v>41</v>
       </c>
       <c r="F17" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="G17" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
         <v>84</v>
@@ -1847,7 +1934,7 @@
         <v>78</v>
       </c>
       <c r="F18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G18" t="s">
         <v>9</v>
@@ -1864,39 +1951,39 @@
         <v>84</v>
       </c>
       <c r="D19" t="s">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="F19" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="G19" t="s">
-        <v>63</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="D20" t="s">
-        <v>108</v>
+        <v>60</v>
       </c>
       <c r="E20" t="s">
-        <v>109</v>
+        <v>61</v>
       </c>
       <c r="F20" t="s">
-        <v>112</v>
+        <v>62</v>
       </c>
       <c r="G20" t="s">
-        <v>111</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1907,19 +1994,19 @@
         <v>65</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="D21" t="s">
-        <v>26</v>
+        <v>115</v>
       </c>
       <c r="E21" t="s">
-        <v>27</v>
+        <v>116</v>
       </c>
       <c r="F21" t="s">
-        <v>66</v>
+        <v>119</v>
       </c>
       <c r="G21" t="s">
-        <v>28</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1933,116 +2020,116 @@
         <v>25</v>
       </c>
       <c r="D22" t="s">
-        <v>75</v>
+        <v>108</v>
       </c>
       <c r="E22" t="s">
-        <v>34</v>
+        <v>109</v>
       </c>
       <c r="F22" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
       <c r="G22" t="s">
-        <v>35</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="C23" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="D23" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="E23" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="F23" t="s">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="G23" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s">
         <v>25</v>
       </c>
       <c r="D24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E24" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F24" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="G24" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s">
         <v>84</v>
       </c>
       <c r="D25" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E25" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F25" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G25" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C26" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="D26" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="E26" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="F26" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="G26" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>67</v>
+        <v>101</v>
       </c>
       <c r="B27" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="C27" t="s">
         <v>25</v>
@@ -2054,7 +2141,7 @@
         <v>38</v>
       </c>
       <c r="F27" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G27" t="s">
         <v>39</v>
@@ -2062,87 +2149,156 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>69</v>
+        <v>104</v>
+      </c>
+      <c r="B28" t="s">
+        <v>54</v>
       </c>
       <c r="C28" t="s">
         <v>84</v>
       </c>
       <c r="D28" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="E28" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="F28" t="s">
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="G28" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>69</v>
+        <v>104</v>
+      </c>
+      <c r="B29" t="s">
+        <v>54</v>
       </c>
       <c r="C29" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="D29" t="s">
-        <v>8</v>
+        <v>108</v>
       </c>
       <c r="E29" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="F29" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="G29" t="s">
-        <v>9</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B30" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C30" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="D30" t="s">
-        <v>8</v>
+        <v>77</v>
       </c>
       <c r="E30" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="F30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G30" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" t="s">
+        <v>84</v>
+      </c>
+      <c r="D31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" t="s">
+        <v>70</v>
+      </c>
+      <c r="G31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" t="s">
+        <v>78</v>
+      </c>
+      <c r="F32" t="s">
+        <v>83</v>
+      </c>
+      <c r="G32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>71</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B33" t="s">
         <v>72</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C33" t="s">
+        <v>84</v>
+      </c>
+      <c r="D33" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" t="s">
+        <v>78</v>
+      </c>
+      <c r="F33" t="s">
+        <v>107</v>
+      </c>
+      <c r="G33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" t="s">
+        <v>72</v>
+      </c>
+      <c r="C34" t="s">
         <v>25</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D34" t="s">
         <v>108</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E34" t="s">
         <v>109</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F34" t="s">
         <v>114</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G34" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2156,8 +2312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2442,7 +2598,7 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="str">
         <f>CCD_CRUISE_SUMM_ERR_V!A9</f>
-        <v>HI1101</v>
+        <v>HI1001</v>
       </c>
       <c r="B9" s="2" t="b">
         <f>EXACT(CCD_CRUISE_SUMM_ERR_V!A9,'Database Export'!A9)</f>
@@ -2646,7 +2802,7 @@
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="str">
         <f>CCD_CRUISE_SUMM_ERR_V!A15</f>
-        <v>HI1102</v>
+        <v>HI1101</v>
       </c>
       <c r="B15" s="2" t="b">
         <f>EXACT(CCD_CRUISE_SUMM_ERR_V!A15,'Database Export'!A15)</f>
@@ -2714,7 +2870,7 @@
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="str">
         <f>CCD_CRUISE_SUMM_ERR_V!A17</f>
-        <v>OES0607</v>
+        <v>HI1102</v>
       </c>
       <c r="B17" s="2" t="b">
         <f>EXACT(CCD_CRUISE_SUMM_ERR_V!A17,'Database Export'!A17)</f>
@@ -2748,7 +2904,7 @@
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="str">
         <f>CCD_CRUISE_SUMM_ERR_V!A18</f>
-        <v>OES0706</v>
+        <v>OES0607</v>
       </c>
       <c r="B18" s="2" t="b">
         <f>EXACT(CCD_CRUISE_SUMM_ERR_V!A18,'Database Export'!A18)</f>
@@ -2816,7 +2972,7 @@
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="str">
         <f>CCD_CRUISE_SUMM_ERR_V!A20</f>
-        <v>RL-17-05</v>
+        <v>OES0706</v>
       </c>
       <c r="B20" s="2" t="b">
         <f>EXACT(CCD_CRUISE_SUMM_ERR_V!A20,'Database Export'!A20)</f>
@@ -2918,7 +3074,7 @@
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="str">
         <f>CCD_CRUISE_SUMM_ERR_V!A23</f>
-        <v>SE-04-11</v>
+        <v>RL-17-05</v>
       </c>
       <c r="B23" s="2" t="b">
         <f>EXACT(CCD_CRUISE_SUMM_ERR_V!A23,'Database Export'!A23)</f>
@@ -2952,7 +3108,7 @@
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="str">
         <f>CCD_CRUISE_SUMM_ERR_V!A24</f>
-        <v>SE-04-11</v>
+        <v>RL-17-05</v>
       </c>
       <c r="B24" s="2" t="b">
         <f>EXACT(CCD_CRUISE_SUMM_ERR_V!A24,'Database Export'!A24)</f>
@@ -2986,7 +3142,7 @@
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="str">
         <f>CCD_CRUISE_SUMM_ERR_V!A25</f>
-        <v>SE-05-09</v>
+        <v>SE-04-11</v>
       </c>
       <c r="B25" s="2" t="b">
         <f>EXACT(CCD_CRUISE_SUMM_ERR_V!A25,'Database Export'!A25)</f>
@@ -3020,7 +3176,7 @@
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="str">
         <f>CCD_CRUISE_SUMM_ERR_V!A26</f>
-        <v>SE-05-09</v>
+        <v>SE-04-11</v>
       </c>
       <c r="B26" s="2" t="b">
         <f>EXACT(CCD_CRUISE_SUMM_ERR_V!A26,'Database Export'!A26)</f>
@@ -3054,7 +3210,7 @@
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="str">
         <f>CCD_CRUISE_SUMM_ERR_V!A27</f>
-        <v>SE-15-01</v>
+        <v>SE-04-11</v>
       </c>
       <c r="B27" s="2" t="b">
         <f>EXACT(CCD_CRUISE_SUMM_ERR_V!A27,'Database Export'!A27)</f>
@@ -3088,7 +3244,7 @@
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="str">
         <f>CCD_CRUISE_SUMM_ERR_V!A28</f>
-        <v>TC0009 (copy)</v>
+        <v>SE-05-09</v>
       </c>
       <c r="B28" s="2" t="b">
         <f>EXACT(CCD_CRUISE_SUMM_ERR_V!A28,'Database Export'!A28)</f>
@@ -3122,7 +3278,7 @@
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="str">
         <f>CCD_CRUISE_SUMM_ERR_V!A29</f>
-        <v>TC0009 (copy)</v>
+        <v>SE-05-09</v>
       </c>
       <c r="B29" s="2" t="b">
         <f>EXACT(CCD_CRUISE_SUMM_ERR_V!A29,'Database Export'!A29)</f>
@@ -3156,7 +3312,7 @@
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="str">
         <f>CCD_CRUISE_SUMM_ERR_V!A30</f>
-        <v>TC0201</v>
+        <v>SE-15-01</v>
       </c>
       <c r="B30" s="2" t="b">
         <f>EXACT(CCD_CRUISE_SUMM_ERR_V!A30,'Database Export'!A30)</f>
@@ -3190,7 +3346,7 @@
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="str">
         <f>CCD_CRUISE_SUMM_ERR_V!A31</f>
-        <v>TC0201</v>
+        <v>TC0009 (copy)</v>
       </c>
       <c r="B31" s="2" t="b">
         <f>EXACT(CCD_CRUISE_SUMM_ERR_V!A31,'Database Export'!A31)</f>
@@ -3222,9 +3378,9 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+      <c r="A32" s="2" t="str">
         <f>CCD_CRUISE_SUMM_ERR_V!A32</f>
-        <v>0</v>
+        <v>TC0009 (copy)</v>
       </c>
       <c r="B32" s="2" t="b">
         <f>EXACT(CCD_CRUISE_SUMM_ERR_V!A32,'Database Export'!A32)</f>
@@ -3256,9 +3412,9 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+      <c r="A33" s="2" t="str">
         <f>CCD_CRUISE_SUMM_ERR_V!A33</f>
-        <v>0</v>
+        <v>TC0201</v>
       </c>
       <c r="B33" s="2" t="b">
         <f>EXACT(CCD_CRUISE_SUMM_ERR_V!A33,'Database Export'!A33)</f>
@@ -3290,9 +3446,9 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+      <c r="A34" s="2" t="str">
         <f>CCD_CRUISE_SUMM_ERR_V!A34</f>
-        <v>0</v>
+        <v>TC0201</v>
       </c>
       <c r="B34" s="2" t="b">
         <f>EXACT(CCD_CRUISE_SUMM_ERR_V!A34,'Database Export'!A34)</f>

</xml_diff>